<commit_message>
videointegration using vlc module
</commit_message>
<xml_diff>
--- a/videos/New Microsoft Excel Worksheet.xlsx
+++ b/videos/New Microsoft Excel Worksheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship\Tasks\unfairAdvantage\videos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship\Tasks\unfairAdv\unfairAdvantage-Internal\videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A2F265-28A5-47BC-BB04-8359CF4C5CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B548610F-CBC3-4149-9AE1-28B79731B84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="804" yWindow="2280" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>Video Name</t>
   </si>
@@ -112,6 +112,36 @@
   </si>
   <si>
     <t>Video7</t>
+  </si>
+  <si>
+    <t>Time taken to loop through all frames</t>
+  </si>
+  <si>
+    <t>15 seconds</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>09 sec</t>
+  </si>
+  <si>
+    <t>12 sec</t>
+  </si>
+  <si>
+    <t>11 sec</t>
+  </si>
+  <si>
+    <t>10 sec</t>
+  </si>
+  <si>
+    <t>21 sec</t>
+  </si>
+  <si>
+    <t>30 sec</t>
+  </si>
+  <si>
+    <t>Frames per second in python</t>
   </si>
 </sst>
 </file>
@@ -141,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -149,20 +179,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="15">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -210,18 +290,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{650E9AED-3F0D-4CC3-9177-7FC0CFE4C02A}" name="Table1" displayName="Table1" ref="A1:I8" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
-  <autoFilter ref="A1:I8" xr:uid="{650E9AED-3F0D-4CC3-9177-7FC0CFE4C02A}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{77293508-A8EE-472E-9191-23F5EC8C149D}" name="Video Name" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{4E104E36-0710-44EC-86C0-7C72930C1BF7}" name="Video Codec" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{BEE98D49-2861-4284-BA95-D89443EFB31C}" name="Frames" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{93772B7D-1DEC-413E-BDCF-C3430283C641}" name="Resolution" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{1D4B6294-373B-4448-AABF-897CDFB457C4}" name="Facial Landmarks Detected" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{55971646-D374-461A-AC9B-0FF05012857D}" name="Gaze " dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{3649C498-E4AC-48AD-B5B5-8C1D2F324701}" name="Emotion" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{D237E5B0-A516-48FB-848D-30A436CAE5CE}" name="Head" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{2BE2A5A8-9CFB-43A1-AF7C-E4B3C9D023E4}" name="Issue" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{650E9AED-3F0D-4CC3-9177-7FC0CFE4C02A}" name="Table1" displayName="Table1" ref="A1:L8" totalsRowShown="0" headerRowDxfId="0" dataDxfId="14" headerRowBorderDxfId="1">
+  <autoFilter ref="A1:L8" xr:uid="{650E9AED-3F0D-4CC3-9177-7FC0CFE4C02A}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{77293508-A8EE-472E-9191-23F5EC8C149D}" name="Video Name" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{4E104E36-0710-44EC-86C0-7C72930C1BF7}" name="Video Codec" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{BEE98D49-2861-4284-BA95-D89443EFB31C}" name="Frames" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{93772B7D-1DEC-413E-BDCF-C3430283C641}" name="Resolution" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{936CED96-094B-46A3-8730-D28E28AFEDC7}" name="Duration" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{1D4B6294-373B-4448-AABF-897CDFB457C4}" name="Facial Landmarks Detected" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{55971646-D374-461A-AC9B-0FF05012857D}" name="Gaze " dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{3649C498-E4AC-48AD-B5B5-8C1D2F324701}" name="Emotion" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{D237E5B0-A516-48FB-848D-30A436CAE5CE}" name="Head" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{2BE2A5A8-9CFB-43A1-AF7C-E4B3C9D023E4}" name="Issue" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{40D0EBC3-73CB-441F-B1F7-B0A09DED18C8}" name="Time taken to loop through all frames" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{D81D7C4A-5D68-4C7C-ADAE-F5E5371A5539}" name="Frames per second in python" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -490,56 +573,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5546875" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="13.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="13.36328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.90625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.54296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.36328125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -553,13 +646,22 @@
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -573,19 +675,22 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -599,19 +704,22 @@
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -625,19 +733,22 @@
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -651,19 +762,22 @@
         <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="37.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -677,19 +791,22 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="53.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -703,15 +820,18 @@
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>